<commit_message>
Fix small map ID issue
</commit_message>
<xml_diff>
--- a/Supporting Files/Curl maker.xlsx
+++ b/Supporting Files/Curl maker.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKSPACE\LS Sklo\NEW 29052025\OLD BASE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKSPACE\LS Sklo\WEB\Supporting Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCC20D1C-7915-4C5C-BA32-97DF3331A099}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CA99DAA-2FA7-49B9-9F16-A8BCA479A4E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A374BADA-030E-4C20-9DAD-6047E1DD297D}"/>
   </bookViews>
@@ -614,7 +614,7 @@
   <dimension ref="A1:H167"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G165" sqref="G1:H165"/>
+      <selection activeCell="A141" sqref="A141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,7 +711,7 @@
         <v>0</v>
       </c>
       <c r="B7" s="6" t="str">
-        <f>$B$6</f>
+        <f>B6</f>
         <v>https://andistyr.github.io/wu-map/14816/</v>
       </c>
       <c r="C7" t="s">
@@ -737,7 +737,7 @@
         <v>0</v>
       </c>
       <c r="B8" s="6" t="str">
-        <f>$B$6</f>
+        <f>B6</f>
         <v>https://andistyr.github.io/wu-map/14816/</v>
       </c>
       <c r="C8" t="s">
@@ -763,7 +763,7 @@
         <v>0</v>
       </c>
       <c r="B9" s="6" t="str">
-        <f>$B$6</f>
+        <f>B6</f>
         <v>https://andistyr.github.io/wu-map/14816/</v>
       </c>
       <c r="C9" t="s">
@@ -807,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="6" t="str">
-        <f>$B$6</f>
+        <f>B6</f>
         <v>https://andistyr.github.io/wu-map/14816/</v>
       </c>
       <c r="C12" t="s">
@@ -860,7 +860,7 @@
         <v>0</v>
       </c>
       <c r="B16" s="6" t="str">
-        <f t="shared" ref="B16:B23" si="1">$B$6</f>
+        <f>B6</f>
         <v>https://andistyr.github.io/wu-map/14816/</v>
       </c>
       <c r="C16" t="s">
@@ -886,7 +886,7 @@
         <v>0</v>
       </c>
       <c r="B17" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f>B6</f>
         <v>https://andistyr.github.io/wu-map/14816/</v>
       </c>
       <c r="C17" t="s">
@@ -912,7 +912,7 @@
         <v>0</v>
       </c>
       <c r="B18" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f>B6</f>
         <v>https://andistyr.github.io/wu-map/14816/</v>
       </c>
       <c r="C18" t="s">
@@ -938,7 +938,7 @@
         <v>0</v>
       </c>
       <c r="B19" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f>B6</f>
         <v>https://andistyr.github.io/wu-map/14816/</v>
       </c>
       <c r="C19" t="s">
@@ -964,7 +964,7 @@
         <v>0</v>
       </c>
       <c r="B20" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f>B6</f>
         <v>https://andistyr.github.io/wu-map/14816/</v>
       </c>
       <c r="C20" t="s">
@@ -990,7 +990,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f>B6</f>
         <v>https://andistyr.github.io/wu-map/14816/</v>
       </c>
       <c r="C21" t="s">
@@ -1016,7 +1016,7 @@
         <v>0</v>
       </c>
       <c r="B22" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f>B6</f>
         <v>https://andistyr.github.io/wu-map/14816/</v>
       </c>
       <c r="C22" t="s">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="3" t="str">
-        <f t="shared" ref="H22" si="2">CONCATENATE(A22," ",B22,C22," ",D22," ",E22," ",F22)</f>
+        <f t="shared" ref="H22" si="1">CONCATENATE(A22," ",B22,C22," ",D22," ",E22," ",F22)</f>
         <v>curl https://andistyr.github.io/wu-map/14816/images/home_hover.png --output home_hover.png --ssl-no-revoke</v>
       </c>
     </row>
@@ -1042,7 +1042,7 @@
         <v>0</v>
       </c>
       <c r="B23" s="6" t="str">
-        <f t="shared" si="1"/>
+        <f>B6</f>
         <v>https://andistyr.github.io/wu-map/14816/</v>
       </c>
       <c r="C23" t="s">
@@ -1095,7 +1095,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="6" t="str">
-        <f>$B$6</f>
+        <f>B6</f>
         <v>https://andistyr.github.io/wu-map/14816/</v>
       </c>
       <c r="C27" t="s">
@@ -1121,7 +1121,7 @@
         <v>0</v>
       </c>
       <c r="B28" s="6" t="str">
-        <f>$B$6</f>
+        <f>B6</f>
         <v>https://andistyr.github.io/wu-map/14816/</v>
       </c>
       <c r="C28" t="s">
@@ -1147,7 +1147,7 @@
         <v>0</v>
       </c>
       <c r="B29" s="6" t="str">
-        <f>$B$6</f>
+        <f>B6</f>
         <v>https://andistyr.github.io/wu-map/14816/</v>
       </c>
       <c r="C29" t="s">
@@ -1175,7 +1175,7 @@
         <v>13</v>
       </c>
       <c r="H30" s="3" t="str">
-        <f t="shared" ref="H30" si="3">CONCATENATE(A30," ",B30," ",D30," ",E30,"",F30)</f>
+        <f t="shared" ref="H30" si="2">CONCATENATE(A30," ",B30," ",D30," ",E30,"",F30)</f>
         <v xml:space="preserve">   </v>
       </c>
     </row>
@@ -1278,7 +1278,7 @@
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="3" t="str">
-        <f t="shared" ref="H40:H63" si="4">CONCATENATE(A40," ",B40,C40," ",D40," ",E40," ",F40)</f>
+        <f t="shared" ref="H40:H43" si="3">CONCATENATE(A40," ",B40,C40," ",D40," ",E40," ",F40)</f>
         <v>curl https://andistyr.github.io/wu-map/14821//index.html --output index.html --ssl-no-revoke</v>
       </c>
     </row>
@@ -1287,8 +1287,8 @@
         <v>0</v>
       </c>
       <c r="B41" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B40</f>
+        <v>https://andistyr.github.io/wu-map/14821/</v>
       </c>
       <c r="C41" t="s">
         <v>25</v>
@@ -1304,8 +1304,8 @@
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>curl https://andistyr.github.io/wu-map/14816//map.js --output map.js --ssl-no-revoke</v>
+        <f t="shared" si="3"/>
+        <v>curl https://andistyr.github.io/wu-map/14821//map.js --output map.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -1313,8 +1313,8 @@
         <v>0</v>
       </c>
       <c r="B42" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B40</f>
+        <v>https://andistyr.github.io/wu-map/14821/</v>
       </c>
       <c r="C42" t="s">
         <v>26</v>
@@ -1330,8 +1330,8 @@
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>curl https://andistyr.github.io/wu-map/14816//removegoogle.js --output removegoogle.js --ssl-no-revoke</v>
+        <f t="shared" si="3"/>
+        <v>curl https://andistyr.github.io/wu-map/14821//removegoogle.js --output removegoogle.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -1339,8 +1339,8 @@
         <v>0</v>
       </c>
       <c r="B43" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B40</f>
+        <v>https://andistyr.github.io/wu-map/14821/</v>
       </c>
       <c r="C43" t="s">
         <v>27</v>
@@ -1356,8 +1356,8 @@
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="3" t="str">
-        <f t="shared" si="4"/>
-        <v>curl https://andistyr.github.io/wu-map/14816//style.css --output style.css --ssl-no-revoke</v>
+        <f t="shared" si="3"/>
+        <v>curl https://andistyr.github.io/wu-map/14821//style.css --output style.css --ssl-no-revoke</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
@@ -1383,8 +1383,8 @@
         <v>0</v>
       </c>
       <c r="B46" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B40</f>
+        <v>https://andistyr.github.io/wu-map/14821/</v>
       </c>
       <c r="C46" t="s">
         <v>30</v>
@@ -1400,8 +1400,8 @@
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="3" t="str">
-        <f t="shared" ref="H46:H67" si="5">CONCATENATE(A46," ",B46,C46," ",D46," ",E46," ",F46)</f>
-        <v>curl https://andistyr.github.io/wu-map/14816/css/roboto.css --output roboto.css --ssl-no-revoke</v>
+        <f t="shared" ref="H46" si="4">CONCATENATE(A46," ",B46,C46," ",D46," ",E46," ",F46)</f>
+        <v>curl https://andistyr.github.io/wu-map/14821/css/roboto.css --output roboto.css --ssl-no-revoke</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -1436,8 +1436,8 @@
         <v>0</v>
       </c>
       <c r="B50" s="6" t="str">
-        <f t="shared" ref="B50:B57" si="6">$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B40</f>
+        <v>https://andistyr.github.io/wu-map/14821/</v>
       </c>
       <c r="C50" t="s">
         <v>31</v>
@@ -1453,8 +1453,8 @@
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="3" t="str">
-        <f t="shared" ref="H50:H67" si="7">CONCATENATE(A50," ",B50,C50," ",D50," ",E50," ",F50)</f>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/deed_large.png --output deed_large.png --ssl-no-revoke</v>
+        <f t="shared" ref="H50:H57" si="5">CONCATENATE(A50," ",B50,C50," ",D50," ",E50," ",F50)</f>
+        <v>curl https://andistyr.github.io/wu-map/14821/images/deed_large.png --output deed_large.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -1462,8 +1462,8 @@
         <v>0</v>
       </c>
       <c r="B51" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B40</f>
+        <v>https://andistyr.github.io/wu-map/14821/</v>
       </c>
       <c r="C51" t="s">
         <v>32</v>
@@ -1479,8 +1479,8 @@
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/deed_small.png --output deed_small.png --ssl-no-revoke</v>
+        <f t="shared" si="5"/>
+        <v>curl https://andistyr.github.io/wu-map/14821/images/deed_small.png --output deed_small.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -1488,8 +1488,8 @@
         <v>0</v>
       </c>
       <c r="B52" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B40</f>
+        <v>https://andistyr.github.io/wu-map/14821/</v>
       </c>
       <c r="C52" t="s">
         <v>33</v>
@@ -1505,8 +1505,8 @@
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/deed_solo.png --output deed_solo.png --ssl-no-revoke</v>
+        <f t="shared" si="5"/>
+        <v>curl https://andistyr.github.io/wu-map/14821/images/deed_solo.png --output deed_solo.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -1514,8 +1514,8 @@
         <v>0</v>
       </c>
       <c r="B53" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B40</f>
+        <v>https://andistyr.github.io/wu-map/14821/</v>
       </c>
       <c r="C53" t="s">
         <v>34</v>
@@ -1531,8 +1531,8 @@
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/guard_tower.png --output guard_tower.png --ssl-no-revoke</v>
+        <f t="shared" si="5"/>
+        <v>curl https://andistyr.github.io/wu-map/14821/images/guard_tower.png --output guard_tower.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -1540,8 +1540,8 @@
         <v>0</v>
       </c>
       <c r="B54" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B40</f>
+        <v>https://andistyr.github.io/wu-map/14821/</v>
       </c>
       <c r="C54" t="s">
         <v>35</v>
@@ -1557,8 +1557,8 @@
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/poi.png --output poi.png --ssl-no-revoke</v>
+        <f t="shared" si="5"/>
+        <v>curl https://andistyr.github.io/wu-map/14821/images/poi.png --output poi.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
@@ -1566,8 +1566,8 @@
         <v>0</v>
       </c>
       <c r="B55" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B40</f>
+        <v>https://andistyr.github.io/wu-map/14821/</v>
       </c>
       <c r="C55" t="s">
         <v>44</v>
@@ -1583,8 +1583,8 @@
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/home_on.png --output home_on.png --ssl-no-revoke</v>
+        <f t="shared" si="5"/>
+        <v>curl https://andistyr.github.io/wu-map/14821/images/home_on.png --output home_on.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -1592,8 +1592,8 @@
         <v>0</v>
       </c>
       <c r="B56" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B40</f>
+        <v>https://andistyr.github.io/wu-map/14821/</v>
       </c>
       <c r="C56" t="s">
         <v>49</v>
@@ -1609,8 +1609,8 @@
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/home_hover.png --output home_hover.png --ssl-no-revoke</v>
+        <f t="shared" si="5"/>
+        <v>curl https://andistyr.github.io/wu-map/14821/images/home_hover.png --output home_hover.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -1618,8 +1618,8 @@
         <v>0</v>
       </c>
       <c r="B57" s="6" t="str">
-        <f t="shared" si="6"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B40</f>
+        <v>https://andistyr.github.io/wu-map/14821/</v>
       </c>
       <c r="C57" t="s">
         <v>45</v>
@@ -1635,8 +1635,8 @@
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="3" t="str">
-        <f t="shared" si="7"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/home_off.png --output home_off.png --ssl-no-revoke</v>
+        <f t="shared" si="5"/>
+        <v>curl https://andistyr.github.io/wu-map/14821/images/home_off.png --output home_off.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -1671,8 +1671,8 @@
         <v>0</v>
       </c>
       <c r="B61" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B40</f>
+        <v>https://andistyr.github.io/wu-map/14821/</v>
       </c>
       <c r="C61" t="s">
         <v>36</v>
@@ -1688,8 +1688,8 @@
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="3" t="str">
-        <f t="shared" ref="H61:H67" si="8">CONCATENATE(A61," ",B61,C61," ",D61," ",E61," ",F61)</f>
-        <v>curl https://andistyr.github.io/wu-map/14816/scipts/cookies.min.js --output cookies.min.js --ssl-no-revoke</v>
+        <f t="shared" ref="H61:H63" si="6">CONCATENATE(A61," ",B61,C61," ",D61," ",E61," ",F61)</f>
+        <v>curl https://andistyr.github.io/wu-map/14821/scipts/cookies.min.js --output cookies.min.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -1697,8 +1697,8 @@
         <v>0</v>
       </c>
       <c r="B62" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B40</f>
+        <v>https://andistyr.github.io/wu-map/14821/</v>
       </c>
       <c r="C62" t="s">
         <v>37</v>
@@ -1714,8 +1714,8 @@
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/scipts/jquery.min.js --output jquery.min.js --ssl-no-revoke</v>
+        <f t="shared" si="6"/>
+        <v>curl https://andistyr.github.io/wu-map/14821/scipts/jquery.min.js --output jquery.min.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -1723,8 +1723,8 @@
         <v>0</v>
       </c>
       <c r="B63" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B40</f>
+        <v>https://andistyr.github.io/wu-map/14821/</v>
       </c>
       <c r="C63" t="s">
         <v>38</v>
@@ -1740,8 +1740,8 @@
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="3" t="str">
-        <f t="shared" si="8"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/scipts/transparency.min.js --output transparency.min.js --ssl-no-revoke</v>
+        <f t="shared" si="6"/>
+        <v>curl https://andistyr.github.io/wu-map/14821/scipts/transparency.min.js --output transparency.min.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -1751,7 +1751,7 @@
         <v>13</v>
       </c>
       <c r="H64" s="3" t="str">
-        <f t="shared" ref="H64" si="9">CONCATENATE(A64," ",B64," ",D64," ",E64,"",F64)</f>
+        <f t="shared" ref="H64" si="7">CONCATENATE(A64," ",B64," ",D64," ",E64,"",F64)</f>
         <v xml:space="preserve">   </v>
       </c>
     </row>
@@ -1849,7 +1849,7 @@
       </c>
       <c r="G74" s="2"/>
       <c r="H74" s="3" t="str">
-        <f t="shared" ref="H74:H97" si="10">CONCATENATE(A74," ",B74,C74," ",D74," ",E74," ",F74)</f>
+        <f t="shared" ref="H74:H77" si="8">CONCATENATE(A74," ",B74,C74," ",D74," ",E74," ",F74)</f>
         <v>curl https://andistyr.github.io/wu-map/14818//index.html --output index.html --ssl-no-revoke</v>
       </c>
     </row>
@@ -1858,8 +1858,8 @@
         <v>0</v>
       </c>
       <c r="B75" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B74</f>
+        <v>https://andistyr.github.io/wu-map/14818/</v>
       </c>
       <c r="C75" t="s">
         <v>25</v>
@@ -1875,8 +1875,8 @@
       </c>
       <c r="G75" s="2"/>
       <c r="H75" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>curl https://andistyr.github.io/wu-map/14816//map.js --output map.js --ssl-no-revoke</v>
+        <f t="shared" si="8"/>
+        <v>curl https://andistyr.github.io/wu-map/14818//map.js --output map.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -1884,8 +1884,8 @@
         <v>0</v>
       </c>
       <c r="B76" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B74</f>
+        <v>https://andistyr.github.io/wu-map/14818/</v>
       </c>
       <c r="C76" t="s">
         <v>26</v>
@@ -1901,8 +1901,8 @@
       </c>
       <c r="G76" s="2"/>
       <c r="H76" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>curl https://andistyr.github.io/wu-map/14816//removegoogle.js --output removegoogle.js --ssl-no-revoke</v>
+        <f t="shared" si="8"/>
+        <v>curl https://andistyr.github.io/wu-map/14818//removegoogle.js --output removegoogle.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
@@ -1910,8 +1910,8 @@
         <v>0</v>
       </c>
       <c r="B77" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B74</f>
+        <v>https://andistyr.github.io/wu-map/14818/</v>
       </c>
       <c r="C77" t="s">
         <v>27</v>
@@ -1927,8 +1927,8 @@
       </c>
       <c r="G77" s="2"/>
       <c r="H77" s="3" t="str">
-        <f t="shared" si="10"/>
-        <v>curl https://andistyr.github.io/wu-map/14816//style.css --output style.css --ssl-no-revoke</v>
+        <f t="shared" si="8"/>
+        <v>curl https://andistyr.github.io/wu-map/14818//style.css --output style.css --ssl-no-revoke</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -1954,8 +1954,8 @@
         <v>0</v>
       </c>
       <c r="B80" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B74</f>
+        <v>https://andistyr.github.io/wu-map/14818/</v>
       </c>
       <c r="C80" t="s">
         <v>30</v>
@@ -1971,8 +1971,8 @@
       </c>
       <c r="G80" s="2"/>
       <c r="H80" s="3" t="str">
-        <f t="shared" ref="H80:H101" si="11">CONCATENATE(A80," ",B80,C80," ",D80," ",E80," ",F80)</f>
-        <v>curl https://andistyr.github.io/wu-map/14816/css/roboto.css --output roboto.css --ssl-no-revoke</v>
+        <f t="shared" ref="H80" si="9">CONCATENATE(A80," ",B80,C80," ",D80," ",E80," ",F80)</f>
+        <v>curl https://andistyr.github.io/wu-map/14818/css/roboto.css --output roboto.css --ssl-no-revoke</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
@@ -2007,8 +2007,8 @@
         <v>0</v>
       </c>
       <c r="B84" s="6" t="str">
-        <f t="shared" ref="B84:B91" si="12">$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B74</f>
+        <v>https://andistyr.github.io/wu-map/14818/</v>
       </c>
       <c r="C84" t="s">
         <v>31</v>
@@ -2024,8 +2024,8 @@
       </c>
       <c r="G84" s="2"/>
       <c r="H84" s="3" t="str">
-        <f t="shared" ref="H84:H101" si="13">CONCATENATE(A84," ",B84,C84," ",D84," ",E84," ",F84)</f>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/deed_large.png --output deed_large.png --ssl-no-revoke</v>
+        <f t="shared" ref="H84:H91" si="10">CONCATENATE(A84," ",B84,C84," ",D84," ",E84," ",F84)</f>
+        <v>curl https://andistyr.github.io/wu-map/14818/images/deed_large.png --output deed_large.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
@@ -2033,8 +2033,8 @@
         <v>0</v>
       </c>
       <c r="B85" s="6" t="str">
-        <f t="shared" si="12"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B74</f>
+        <v>https://andistyr.github.io/wu-map/14818/</v>
       </c>
       <c r="C85" t="s">
         <v>32</v>
@@ -2050,8 +2050,8 @@
       </c>
       <c r="G85" s="2"/>
       <c r="H85" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/deed_small.png --output deed_small.png --ssl-no-revoke</v>
+        <f t="shared" si="10"/>
+        <v>curl https://andistyr.github.io/wu-map/14818/images/deed_small.png --output deed_small.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.25">
@@ -2059,8 +2059,8 @@
         <v>0</v>
       </c>
       <c r="B86" s="6" t="str">
-        <f t="shared" si="12"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B74</f>
+        <v>https://andistyr.github.io/wu-map/14818/</v>
       </c>
       <c r="C86" t="s">
         <v>33</v>
@@ -2076,8 +2076,8 @@
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/deed_solo.png --output deed_solo.png --ssl-no-revoke</v>
+        <f t="shared" si="10"/>
+        <v>curl https://andistyr.github.io/wu-map/14818/images/deed_solo.png --output deed_solo.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -2085,8 +2085,8 @@
         <v>0</v>
       </c>
       <c r="B87" s="6" t="str">
-        <f t="shared" si="12"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B74</f>
+        <v>https://andistyr.github.io/wu-map/14818/</v>
       </c>
       <c r="C87" t="s">
         <v>34</v>
@@ -2102,8 +2102,8 @@
       </c>
       <c r="G87" s="2"/>
       <c r="H87" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/guard_tower.png --output guard_tower.png --ssl-no-revoke</v>
+        <f t="shared" si="10"/>
+        <v>curl https://andistyr.github.io/wu-map/14818/images/guard_tower.png --output guard_tower.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
@@ -2111,8 +2111,8 @@
         <v>0</v>
       </c>
       <c r="B88" s="6" t="str">
-        <f t="shared" si="12"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B74</f>
+        <v>https://andistyr.github.io/wu-map/14818/</v>
       </c>
       <c r="C88" t="s">
         <v>35</v>
@@ -2128,8 +2128,8 @@
       </c>
       <c r="G88" s="2"/>
       <c r="H88" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/poi.png --output poi.png --ssl-no-revoke</v>
+        <f t="shared" si="10"/>
+        <v>curl https://andistyr.github.io/wu-map/14818/images/poi.png --output poi.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.25">
@@ -2137,8 +2137,8 @@
         <v>0</v>
       </c>
       <c r="B89" s="6" t="str">
-        <f t="shared" si="12"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B74</f>
+        <v>https://andistyr.github.io/wu-map/14818/</v>
       </c>
       <c r="C89" t="s">
         <v>44</v>
@@ -2154,8 +2154,8 @@
       </c>
       <c r="G89" s="2"/>
       <c r="H89" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/home_on.png --output home_on.png --ssl-no-revoke</v>
+        <f t="shared" si="10"/>
+        <v>curl https://andistyr.github.io/wu-map/14818/images/home_on.png --output home_on.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -2163,8 +2163,8 @@
         <v>0</v>
       </c>
       <c r="B90" s="6" t="str">
-        <f t="shared" si="12"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B74</f>
+        <v>https://andistyr.github.io/wu-map/14818/</v>
       </c>
       <c r="C90" t="s">
         <v>49</v>
@@ -2180,8 +2180,8 @@
       </c>
       <c r="G90" s="2"/>
       <c r="H90" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/home_hover.png --output home_hover.png --ssl-no-revoke</v>
+        <f t="shared" si="10"/>
+        <v>curl https://andistyr.github.io/wu-map/14818/images/home_hover.png --output home_hover.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -2189,8 +2189,8 @@
         <v>0</v>
       </c>
       <c r="B91" s="6" t="str">
-        <f t="shared" si="12"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B74</f>
+        <v>https://andistyr.github.io/wu-map/14818/</v>
       </c>
       <c r="C91" t="s">
         <v>45</v>
@@ -2206,8 +2206,8 @@
       </c>
       <c r="G91" s="2"/>
       <c r="H91" s="3" t="str">
-        <f t="shared" si="13"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/home_off.png --output home_off.png --ssl-no-revoke</v>
+        <f t="shared" si="10"/>
+        <v>curl https://andistyr.github.io/wu-map/14818/images/home_off.png --output home_off.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -2242,8 +2242,8 @@
         <v>0</v>
       </c>
       <c r="B95" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B74</f>
+        <v>https://andistyr.github.io/wu-map/14818/</v>
       </c>
       <c r="C95" t="s">
         <v>36</v>
@@ -2259,8 +2259,8 @@
       </c>
       <c r="G95" s="2"/>
       <c r="H95" s="3" t="str">
-        <f t="shared" ref="H95:H101" si="14">CONCATENATE(A95," ",B95,C95," ",D95," ",E95," ",F95)</f>
-        <v>curl https://andistyr.github.io/wu-map/14816/scipts/cookies.min.js --output cookies.min.js --ssl-no-revoke</v>
+        <f t="shared" ref="H95:H97" si="11">CONCATENATE(A95," ",B95,C95," ",D95," ",E95," ",F95)</f>
+        <v>curl https://andistyr.github.io/wu-map/14818/scipts/cookies.min.js --output cookies.min.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -2268,8 +2268,8 @@
         <v>0</v>
       </c>
       <c r="B96" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B74</f>
+        <v>https://andistyr.github.io/wu-map/14818/</v>
       </c>
       <c r="C96" t="s">
         <v>37</v>
@@ -2285,8 +2285,8 @@
       </c>
       <c r="G96" s="2"/>
       <c r="H96" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/scipts/jquery.min.js --output jquery.min.js --ssl-no-revoke</v>
+        <f t="shared" si="11"/>
+        <v>curl https://andistyr.github.io/wu-map/14818/scipts/jquery.min.js --output jquery.min.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -2294,8 +2294,8 @@
         <v>0</v>
       </c>
       <c r="B97" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B74</f>
+        <v>https://andistyr.github.io/wu-map/14818/</v>
       </c>
       <c r="C97" t="s">
         <v>38</v>
@@ -2311,8 +2311,8 @@
       </c>
       <c r="G97" s="2"/>
       <c r="H97" s="3" t="str">
-        <f t="shared" si="14"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/scipts/transparency.min.js --output transparency.min.js --ssl-no-revoke</v>
+        <f t="shared" si="11"/>
+        <v>curl https://andistyr.github.io/wu-map/14818/scipts/transparency.min.js --output transparency.min.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -2322,7 +2322,7 @@
         <v>13</v>
       </c>
       <c r="H98" s="3" t="str">
-        <f t="shared" ref="H98" si="15">CONCATENATE(A98," ",B98," ",D98," ",E98,"",F98)</f>
+        <f t="shared" ref="H98" si="12">CONCATENATE(A98," ",B98," ",D98," ",E98,"",F98)</f>
         <v xml:space="preserve">   </v>
       </c>
     </row>
@@ -2418,7 +2418,7 @@
       </c>
       <c r="G107" s="2"/>
       <c r="H107" s="3" t="str">
-        <f t="shared" ref="H107:H130" si="16">CONCATENATE(A107," ",B107,C107," ",D107," ",E107," ",F107)</f>
+        <f t="shared" ref="H107:H110" si="13">CONCATENATE(A107," ",B107,C107," ",D107," ",E107," ",F107)</f>
         <v>curl https://andistyr.github.io/wu-map/14901//index.html --output index.html --ssl-no-revoke</v>
       </c>
     </row>
@@ -2427,8 +2427,8 @@
         <v>0</v>
       </c>
       <c r="B108" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B107</f>
+        <v>https://andistyr.github.io/wu-map/14901/</v>
       </c>
       <c r="C108" t="s">
         <v>25</v>
@@ -2444,8 +2444,8 @@
       </c>
       <c r="G108" s="2"/>
       <c r="H108" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v>curl https://andistyr.github.io/wu-map/14816//map.js --output map.js --ssl-no-revoke</v>
+        <f t="shared" si="13"/>
+        <v>curl https://andistyr.github.io/wu-map/14901//map.js --output map.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -2453,8 +2453,8 @@
         <v>0</v>
       </c>
       <c r="B109" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B107</f>
+        <v>https://andistyr.github.io/wu-map/14901/</v>
       </c>
       <c r="C109" t="s">
         <v>26</v>
@@ -2470,8 +2470,8 @@
       </c>
       <c r="G109" s="2"/>
       <c r="H109" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v>curl https://andistyr.github.io/wu-map/14816//removegoogle.js --output removegoogle.js --ssl-no-revoke</v>
+        <f t="shared" si="13"/>
+        <v>curl https://andistyr.github.io/wu-map/14901//removegoogle.js --output removegoogle.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -2479,8 +2479,8 @@
         <v>0</v>
       </c>
       <c r="B110" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B107</f>
+        <v>https://andistyr.github.io/wu-map/14901/</v>
       </c>
       <c r="C110" t="s">
         <v>27</v>
@@ -2496,8 +2496,8 @@
       </c>
       <c r="G110" s="2"/>
       <c r="H110" s="3" t="str">
-        <f t="shared" si="16"/>
-        <v>curl https://andistyr.github.io/wu-map/14816//style.css --output style.css --ssl-no-revoke</v>
+        <f t="shared" si="13"/>
+        <v>curl https://andistyr.github.io/wu-map/14901//style.css --output style.css --ssl-no-revoke</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
@@ -2523,8 +2523,8 @@
         <v>0</v>
       </c>
       <c r="B113" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B107</f>
+        <v>https://andistyr.github.io/wu-map/14901/</v>
       </c>
       <c r="C113" t="s">
         <v>30</v>
@@ -2540,8 +2540,8 @@
       </c>
       <c r="G113" s="2"/>
       <c r="H113" s="3" t="str">
-        <f t="shared" ref="H113:H134" si="17">CONCATENATE(A113," ",B113,C113," ",D113," ",E113," ",F113)</f>
-        <v>curl https://andistyr.github.io/wu-map/14816/css/roboto.css --output roboto.css --ssl-no-revoke</v>
+        <f t="shared" ref="H113" si="14">CONCATENATE(A113," ",B113,C113," ",D113," ",E113," ",F113)</f>
+        <v>curl https://andistyr.github.io/wu-map/14901/css/roboto.css --output roboto.css --ssl-no-revoke</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -2576,8 +2576,8 @@
         <v>0</v>
       </c>
       <c r="B117" s="6" t="str">
-        <f t="shared" ref="B117:B124" si="18">$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B107</f>
+        <v>https://andistyr.github.io/wu-map/14901/</v>
       </c>
       <c r="C117" t="s">
         <v>31</v>
@@ -2593,8 +2593,8 @@
       </c>
       <c r="G117" s="2"/>
       <c r="H117" s="3" t="str">
-        <f t="shared" ref="H117:H134" si="19">CONCATENATE(A117," ",B117,C117," ",D117," ",E117," ",F117)</f>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/deed_large.png --output deed_large.png --ssl-no-revoke</v>
+        <f t="shared" ref="H117:H124" si="15">CONCATENATE(A117," ",B117,C117," ",D117," ",E117," ",F117)</f>
+        <v>curl https://andistyr.github.io/wu-map/14901/images/deed_large.png --output deed_large.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -2602,8 +2602,8 @@
         <v>0</v>
       </c>
       <c r="B118" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B107</f>
+        <v>https://andistyr.github.io/wu-map/14901/</v>
       </c>
       <c r="C118" t="s">
         <v>32</v>
@@ -2619,8 +2619,8 @@
       </c>
       <c r="G118" s="2"/>
       <c r="H118" s="3" t="str">
-        <f t="shared" si="19"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/deed_small.png --output deed_small.png --ssl-no-revoke</v>
+        <f t="shared" si="15"/>
+        <v>curl https://andistyr.github.io/wu-map/14901/images/deed_small.png --output deed_small.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.25">
@@ -2628,8 +2628,8 @@
         <v>0</v>
       </c>
       <c r="B119" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B107</f>
+        <v>https://andistyr.github.io/wu-map/14901/</v>
       </c>
       <c r="C119" t="s">
         <v>33</v>
@@ -2645,8 +2645,8 @@
       </c>
       <c r="G119" s="2"/>
       <c r="H119" s="3" t="str">
-        <f t="shared" si="19"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/deed_solo.png --output deed_solo.png --ssl-no-revoke</v>
+        <f t="shared" si="15"/>
+        <v>curl https://andistyr.github.io/wu-map/14901/images/deed_solo.png --output deed_solo.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -2654,8 +2654,8 @@
         <v>0</v>
       </c>
       <c r="B120" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B107</f>
+        <v>https://andistyr.github.io/wu-map/14901/</v>
       </c>
       <c r="C120" t="s">
         <v>34</v>
@@ -2671,8 +2671,8 @@
       </c>
       <c r="G120" s="2"/>
       <c r="H120" s="3" t="str">
-        <f t="shared" si="19"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/guard_tower.png --output guard_tower.png --ssl-no-revoke</v>
+        <f t="shared" si="15"/>
+        <v>curl https://andistyr.github.io/wu-map/14901/images/guard_tower.png --output guard_tower.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -2680,8 +2680,8 @@
         <v>0</v>
       </c>
       <c r="B121" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B107</f>
+        <v>https://andistyr.github.io/wu-map/14901/</v>
       </c>
       <c r="C121" t="s">
         <v>35</v>
@@ -2697,8 +2697,8 @@
       </c>
       <c r="G121" s="2"/>
       <c r="H121" s="3" t="str">
-        <f t="shared" si="19"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/poi.png --output poi.png --ssl-no-revoke</v>
+        <f t="shared" si="15"/>
+        <v>curl https://andistyr.github.io/wu-map/14901/images/poi.png --output poi.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.25">
@@ -2706,8 +2706,8 @@
         <v>0</v>
       </c>
       <c r="B122" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B107</f>
+        <v>https://andistyr.github.io/wu-map/14901/</v>
       </c>
       <c r="C122" t="s">
         <v>44</v>
@@ -2723,8 +2723,8 @@
       </c>
       <c r="G122" s="2"/>
       <c r="H122" s="3" t="str">
-        <f t="shared" si="19"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/home_on.png --output home_on.png --ssl-no-revoke</v>
+        <f t="shared" si="15"/>
+        <v>curl https://andistyr.github.io/wu-map/14901/images/home_on.png --output home_on.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -2732,8 +2732,8 @@
         <v>0</v>
       </c>
       <c r="B123" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B107</f>
+        <v>https://andistyr.github.io/wu-map/14901/</v>
       </c>
       <c r="C123" t="s">
         <v>49</v>
@@ -2749,8 +2749,8 @@
       </c>
       <c r="G123" s="2"/>
       <c r="H123" s="3" t="str">
-        <f t="shared" si="19"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/home_hover.png --output home_hover.png --ssl-no-revoke</v>
+        <f t="shared" si="15"/>
+        <v>curl https://andistyr.github.io/wu-map/14901/images/home_hover.png --output home_hover.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -2758,8 +2758,8 @@
         <v>0</v>
       </c>
       <c r="B124" s="6" t="str">
-        <f t="shared" si="18"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B107</f>
+        <v>https://andistyr.github.io/wu-map/14901/</v>
       </c>
       <c r="C124" t="s">
         <v>45</v>
@@ -2775,8 +2775,8 @@
       </c>
       <c r="G124" s="2"/>
       <c r="H124" s="3" t="str">
-        <f t="shared" si="19"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/home_off.png --output home_off.png --ssl-no-revoke</v>
+        <f t="shared" si="15"/>
+        <v>curl https://andistyr.github.io/wu-map/14901/images/home_off.png --output home_off.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -2811,8 +2811,8 @@
         <v>0</v>
       </c>
       <c r="B128" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B107</f>
+        <v>https://andistyr.github.io/wu-map/14901/</v>
       </c>
       <c r="C128" t="s">
         <v>36</v>
@@ -2828,8 +2828,8 @@
       </c>
       <c r="G128" s="2"/>
       <c r="H128" s="3" t="str">
-        <f t="shared" ref="H128:H134" si="20">CONCATENATE(A128," ",B128,C128," ",D128," ",E128," ",F128)</f>
-        <v>curl https://andistyr.github.io/wu-map/14816/scipts/cookies.min.js --output cookies.min.js --ssl-no-revoke</v>
+        <f t="shared" ref="H128:H130" si="16">CONCATENATE(A128," ",B128,C128," ",D128," ",E128," ",F128)</f>
+        <v>curl https://andistyr.github.io/wu-map/14901/scipts/cookies.min.js --output cookies.min.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -2837,8 +2837,8 @@
         <v>0</v>
       </c>
       <c r="B129" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B107</f>
+        <v>https://andistyr.github.io/wu-map/14901/</v>
       </c>
       <c r="C129" t="s">
         <v>37</v>
@@ -2854,8 +2854,8 @@
       </c>
       <c r="G129" s="2"/>
       <c r="H129" s="3" t="str">
-        <f t="shared" si="20"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/scipts/jquery.min.js --output jquery.min.js --ssl-no-revoke</v>
+        <f t="shared" si="16"/>
+        <v>curl https://andistyr.github.io/wu-map/14901/scipts/jquery.min.js --output jquery.min.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.25">
@@ -2863,8 +2863,8 @@
         <v>0</v>
       </c>
       <c r="B130" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B107</f>
+        <v>https://andistyr.github.io/wu-map/14901/</v>
       </c>
       <c r="C130" t="s">
         <v>38</v>
@@ -2880,8 +2880,8 @@
       </c>
       <c r="G130" s="2"/>
       <c r="H130" s="3" t="str">
-        <f t="shared" si="20"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/scipts/transparency.min.js --output transparency.min.js --ssl-no-revoke</v>
+        <f t="shared" si="16"/>
+        <v>curl https://andistyr.github.io/wu-map/14901/scipts/transparency.min.js --output transparency.min.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -2891,7 +2891,7 @@
         <v>13</v>
       </c>
       <c r="H131" s="3" t="str">
-        <f t="shared" ref="H131" si="21">CONCATENATE(A131," ",B131," ",D131," ",E131,"",F131)</f>
+        <f t="shared" ref="H131" si="17">CONCATENATE(A131," ",B131," ",D131," ",E131,"",F131)</f>
         <v xml:space="preserve">   </v>
       </c>
     </row>
@@ -2987,7 +2987,7 @@
       </c>
       <c r="G140" s="2"/>
       <c r="H140" s="3" t="str">
-        <f t="shared" ref="H140:H163" si="22">CONCATENATE(A140," ",B140,C140," ",D140," ",E140," ",F140)</f>
+        <f t="shared" ref="H140:H143" si="18">CONCATENATE(A140," ",B140,C140," ",D140," ",E140," ",F140)</f>
         <v>curl https://andistyr.github.io/wu-map/14852//index.html --output index.html --ssl-no-revoke</v>
       </c>
     </row>
@@ -2996,8 +2996,8 @@
         <v>0</v>
       </c>
       <c r="B141" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B140</f>
+        <v>https://andistyr.github.io/wu-map/14852/</v>
       </c>
       <c r="C141" t="s">
         <v>25</v>
@@ -3013,8 +3013,8 @@
       </c>
       <c r="G141" s="2"/>
       <c r="H141" s="3" t="str">
-        <f t="shared" si="22"/>
-        <v>curl https://andistyr.github.io/wu-map/14816//map.js --output map.js --ssl-no-revoke</v>
+        <f t="shared" si="18"/>
+        <v>curl https://andistyr.github.io/wu-map/14852//map.js --output map.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.25">
@@ -3022,8 +3022,8 @@
         <v>0</v>
       </c>
       <c r="B142" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B140</f>
+        <v>https://andistyr.github.io/wu-map/14852/</v>
       </c>
       <c r="C142" t="s">
         <v>26</v>
@@ -3039,8 +3039,8 @@
       </c>
       <c r="G142" s="2"/>
       <c r="H142" s="3" t="str">
-        <f t="shared" si="22"/>
-        <v>curl https://andistyr.github.io/wu-map/14816//removegoogle.js --output removegoogle.js --ssl-no-revoke</v>
+        <f t="shared" si="18"/>
+        <v>curl https://andistyr.github.io/wu-map/14852//removegoogle.js --output removegoogle.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -3048,8 +3048,8 @@
         <v>0</v>
       </c>
       <c r="B143" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B140</f>
+        <v>https://andistyr.github.io/wu-map/14852/</v>
       </c>
       <c r="C143" t="s">
         <v>27</v>
@@ -3065,8 +3065,8 @@
       </c>
       <c r="G143" s="2"/>
       <c r="H143" s="3" t="str">
-        <f t="shared" si="22"/>
-        <v>curl https://andistyr.github.io/wu-map/14816//style.css --output style.css --ssl-no-revoke</v>
+        <f t="shared" si="18"/>
+        <v>curl https://andistyr.github.io/wu-map/14852//style.css --output style.css --ssl-no-revoke</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -3092,8 +3092,8 @@
         <v>0</v>
       </c>
       <c r="B146" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B140</f>
+        <v>https://andistyr.github.io/wu-map/14852/</v>
       </c>
       <c r="C146" t="s">
         <v>30</v>
@@ -3109,8 +3109,8 @@
       </c>
       <c r="G146" s="2"/>
       <c r="H146" s="3" t="str">
-        <f t="shared" ref="H146:H167" si="23">CONCATENATE(A146," ",B146,C146," ",D146," ",E146," ",F146)</f>
-        <v>curl https://andistyr.github.io/wu-map/14816/css/roboto.css --output roboto.css --ssl-no-revoke</v>
+        <f t="shared" ref="H146" si="19">CONCATENATE(A146," ",B146,C146," ",D146," ",E146," ",F146)</f>
+        <v>curl https://andistyr.github.io/wu-map/14852/css/roboto.css --output roboto.css --ssl-no-revoke</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -3145,8 +3145,8 @@
         <v>0</v>
       </c>
       <c r="B150" s="6" t="str">
-        <f t="shared" ref="B150:B157" si="24">$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B140</f>
+        <v>https://andistyr.github.io/wu-map/14852/</v>
       </c>
       <c r="C150" t="s">
         <v>31</v>
@@ -3162,8 +3162,8 @@
       </c>
       <c r="G150" s="2"/>
       <c r="H150" s="3" t="str">
-        <f t="shared" ref="H150:H167" si="25">CONCATENATE(A150," ",B150,C150," ",D150," ",E150," ",F150)</f>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/deed_large.png --output deed_large.png --ssl-no-revoke</v>
+        <f t="shared" ref="H150:H157" si="20">CONCATENATE(A150," ",B150,C150," ",D150," ",E150," ",F150)</f>
+        <v>curl https://andistyr.github.io/wu-map/14852/images/deed_large.png --output deed_large.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -3171,8 +3171,8 @@
         <v>0</v>
       </c>
       <c r="B151" s="6" t="str">
-        <f t="shared" si="24"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B140</f>
+        <v>https://andistyr.github.io/wu-map/14852/</v>
       </c>
       <c r="C151" t="s">
         <v>32</v>
@@ -3188,8 +3188,8 @@
       </c>
       <c r="G151" s="2"/>
       <c r="H151" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/deed_small.png --output deed_small.png --ssl-no-revoke</v>
+        <f t="shared" si="20"/>
+        <v>curl https://andistyr.github.io/wu-map/14852/images/deed_small.png --output deed_small.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
@@ -3197,8 +3197,8 @@
         <v>0</v>
       </c>
       <c r="B152" s="6" t="str">
-        <f t="shared" si="24"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B140</f>
+        <v>https://andistyr.github.io/wu-map/14852/</v>
       </c>
       <c r="C152" t="s">
         <v>33</v>
@@ -3214,8 +3214,8 @@
       </c>
       <c r="G152" s="2"/>
       <c r="H152" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/deed_solo.png --output deed_solo.png --ssl-no-revoke</v>
+        <f t="shared" si="20"/>
+        <v>curl https://andistyr.github.io/wu-map/14852/images/deed_solo.png --output deed_solo.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -3223,8 +3223,8 @@
         <v>0</v>
       </c>
       <c r="B153" s="6" t="str">
-        <f t="shared" si="24"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B140</f>
+        <v>https://andistyr.github.io/wu-map/14852/</v>
       </c>
       <c r="C153" t="s">
         <v>34</v>
@@ -3240,8 +3240,8 @@
       </c>
       <c r="G153" s="2"/>
       <c r="H153" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/guard_tower.png --output guard_tower.png --ssl-no-revoke</v>
+        <f t="shared" si="20"/>
+        <v>curl https://andistyr.github.io/wu-map/14852/images/guard_tower.png --output guard_tower.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -3249,8 +3249,8 @@
         <v>0</v>
       </c>
       <c r="B154" s="6" t="str">
-        <f t="shared" si="24"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B140</f>
+        <v>https://andistyr.github.io/wu-map/14852/</v>
       </c>
       <c r="C154" t="s">
         <v>35</v>
@@ -3266,8 +3266,8 @@
       </c>
       <c r="G154" s="2"/>
       <c r="H154" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/poi.png --output poi.png --ssl-no-revoke</v>
+        <f t="shared" si="20"/>
+        <v>curl https://andistyr.github.io/wu-map/14852/images/poi.png --output poi.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -3275,8 +3275,8 @@
         <v>0</v>
       </c>
       <c r="B155" s="6" t="str">
-        <f t="shared" si="24"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B140</f>
+        <v>https://andistyr.github.io/wu-map/14852/</v>
       </c>
       <c r="C155" t="s">
         <v>44</v>
@@ -3292,8 +3292,8 @@
       </c>
       <c r="G155" s="2"/>
       <c r="H155" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/home_on.png --output home_on.png --ssl-no-revoke</v>
+        <f t="shared" si="20"/>
+        <v>curl https://andistyr.github.io/wu-map/14852/images/home_on.png --output home_on.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -3301,8 +3301,8 @@
         <v>0</v>
       </c>
       <c r="B156" s="6" t="str">
-        <f t="shared" si="24"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B140</f>
+        <v>https://andistyr.github.io/wu-map/14852/</v>
       </c>
       <c r="C156" t="s">
         <v>49</v>
@@ -3318,8 +3318,8 @@
       </c>
       <c r="G156" s="2"/>
       <c r="H156" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/home_hover.png --output home_hover.png --ssl-no-revoke</v>
+        <f t="shared" si="20"/>
+        <v>curl https://andistyr.github.io/wu-map/14852/images/home_hover.png --output home_hover.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -3327,8 +3327,8 @@
         <v>0</v>
       </c>
       <c r="B157" s="6" t="str">
-        <f t="shared" si="24"/>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B140</f>
+        <v>https://andistyr.github.io/wu-map/14852/</v>
       </c>
       <c r="C157" t="s">
         <v>45</v>
@@ -3344,8 +3344,8 @@
       </c>
       <c r="G157" s="2"/>
       <c r="H157" s="3" t="str">
-        <f t="shared" si="25"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/images/home_off.png --output home_off.png --ssl-no-revoke</v>
+        <f t="shared" si="20"/>
+        <v>curl https://andistyr.github.io/wu-map/14852/images/home_off.png --output home_off.png --ssl-no-revoke</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -3380,8 +3380,8 @@
         <v>0</v>
       </c>
       <c r="B161" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B140</f>
+        <v>https://andistyr.github.io/wu-map/14852/</v>
       </c>
       <c r="C161" t="s">
         <v>36</v>
@@ -3397,8 +3397,8 @@
       </c>
       <c r="G161" s="2"/>
       <c r="H161" s="3" t="str">
-        <f t="shared" ref="H161:H167" si="26">CONCATENATE(A161," ",B161,C161," ",D161," ",E161," ",F161)</f>
-        <v>curl https://andistyr.github.io/wu-map/14816/scipts/cookies.min.js --output cookies.min.js --ssl-no-revoke</v>
+        <f t="shared" ref="H161:H163" si="21">CONCATENATE(A161," ",B161,C161," ",D161," ",E161," ",F161)</f>
+        <v>curl https://andistyr.github.io/wu-map/14852/scipts/cookies.min.js --output cookies.min.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.25">
@@ -3406,8 +3406,8 @@
         <v>0</v>
       </c>
       <c r="B162" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B140</f>
+        <v>https://andistyr.github.io/wu-map/14852/</v>
       </c>
       <c r="C162" t="s">
         <v>37</v>
@@ -3423,8 +3423,8 @@
       </c>
       <c r="G162" s="2"/>
       <c r="H162" s="3" t="str">
-        <f t="shared" si="26"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/scipts/jquery.min.js --output jquery.min.js --ssl-no-revoke</v>
+        <f t="shared" si="21"/>
+        <v>curl https://andistyr.github.io/wu-map/14852/scipts/jquery.min.js --output jquery.min.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -3432,8 +3432,8 @@
         <v>0</v>
       </c>
       <c r="B163" s="6" t="str">
-        <f>$B$6</f>
-        <v>https://andistyr.github.io/wu-map/14816/</v>
+        <f>B140</f>
+        <v>https://andistyr.github.io/wu-map/14852/</v>
       </c>
       <c r="C163" t="s">
         <v>38</v>
@@ -3449,8 +3449,8 @@
       </c>
       <c r="G163" s="2"/>
       <c r="H163" s="3" t="str">
-        <f t="shared" si="26"/>
-        <v>curl https://andistyr.github.io/wu-map/14816/scipts/transparency.min.js --output transparency.min.js --ssl-no-revoke</v>
+        <f t="shared" si="21"/>
+        <v>curl https://andistyr.github.io/wu-map/14852/scipts/transparency.min.js --output transparency.min.js --ssl-no-revoke</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
@@ -3460,7 +3460,7 @@
         <v>13</v>
       </c>
       <c r="H164" s="3" t="str">
-        <f t="shared" ref="H164" si="27">CONCATENATE(A164," ",B164," ",D164," ",E164,"",F164)</f>
+        <f t="shared" ref="H164" si="22">CONCATENATE(A164," ",B164," ",D164," ",E164,"",F164)</f>
         <v xml:space="preserve">   </v>
       </c>
     </row>
@@ -3486,14 +3486,14 @@
   <hyperlinks>
     <hyperlink ref="B6" r:id="rId1" display="https://andistyr.github.io/wu-map/14818/" xr:uid="{4D15660C-6DB0-4418-8DBA-08EB4387B0C0}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{06F2D811-15A0-4D61-A3D1-8B8D91A45405}"/>
-    <hyperlink ref="B40" r:id="rId3" display="https://andistyr.github.io/wu-map/14818/" xr:uid="{85BAD2EC-F3E5-4704-BE37-347E150C6FE4}"/>
-    <hyperlink ref="B37" r:id="rId4" xr:uid="{EA984F3A-2B77-44DB-AAAE-D3AE8B5EF4C7}"/>
-    <hyperlink ref="B74" r:id="rId5" display="https://andistyr.github.io/wu-map/14818/" xr:uid="{FCF81AE7-E395-4448-B54E-E4DAFA9BCC44}"/>
-    <hyperlink ref="B71" r:id="rId6" xr:uid="{E7B0B474-0807-45E4-AF9C-F62CEFA3B1D7}"/>
-    <hyperlink ref="B107" r:id="rId7" display="https://andistyr.github.io/wu-map/14818/" xr:uid="{1D98B125-5AA0-451C-8804-EA5F49BD323C}"/>
-    <hyperlink ref="B104" r:id="rId8" xr:uid="{806685F9-21A2-4C20-991C-E4B08BFAFA37}"/>
-    <hyperlink ref="B140" r:id="rId9" display="https://andistyr.github.io/wu-map/14818/" xr:uid="{8E7C269B-31FD-4CDA-BE6D-F034185E1C14}"/>
-    <hyperlink ref="B137" r:id="rId10" xr:uid="{E55B24DA-ED3A-4BDF-ADC4-72FCA59E85B4}"/>
+    <hyperlink ref="B37" r:id="rId3" xr:uid="{EA984F3A-2B77-44DB-AAAE-D3AE8B5EF4C7}"/>
+    <hyperlink ref="B71" r:id="rId4" xr:uid="{E7B0B474-0807-45E4-AF9C-F62CEFA3B1D7}"/>
+    <hyperlink ref="B104" r:id="rId5" xr:uid="{806685F9-21A2-4C20-991C-E4B08BFAFA37}"/>
+    <hyperlink ref="B137" r:id="rId6" xr:uid="{E55B24DA-ED3A-4BDF-ADC4-72FCA59E85B4}"/>
+    <hyperlink ref="B40" r:id="rId7" display="https://andistyr.github.io/wu-map/14818/" xr:uid="{5DAF6C9B-00EA-4798-A5E8-B9AC8DB0CFB5}"/>
+    <hyperlink ref="B74" r:id="rId8" display="https://andistyr.github.io/wu-map/14818/" xr:uid="{F630E47A-4639-48B6-9E37-44AEF59BBC6B}"/>
+    <hyperlink ref="B107" r:id="rId9" display="https://andistyr.github.io/wu-map/14818/" xr:uid="{124B661E-29DE-4AC7-B0FA-AE3D30A0DEA6}"/>
+    <hyperlink ref="B140" r:id="rId10" display="https://andistyr.github.io/wu-map/14818/" xr:uid="{E6189EE2-A074-4D20-8427-686933D3E28F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId11"/>

</xml_diff>